<commit_message>
Changed name/type of storage device into an optional column
</commit_message>
<xml_diff>
--- a/doc/Batch_Upload_Template.xlsx
+++ b/doc/Batch_Upload_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmattioli\Projects\XNAT-Interact\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96F0C4E-A3BD-4657-BEE4-538D95A655B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DE4112-ACA6-487D-B14B-E43E2877FEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="3930" windowWidth="29040" windowHeight="15720" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
   </bookViews>
@@ -2281,7 +2281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2464,6 +2464,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2889,8 +2898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835E2DA3-F8AB-4F0F-8564-A4EB2F259832}">
   <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2917,7 +2926,7 @@
     <col min="20" max="20" width="11.7109375" style="43" customWidth="1"/>
     <col min="21" max="21" width="9.140625" style="3" customWidth="1"/>
     <col min="22" max="22" width="12.28515625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" style="70" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="105.7109375" style="35" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.28515625" style="43" customWidth="1"/>
     <col min="26" max="34" width="9.140625" style="1" hidden="1" customWidth="1"/>
@@ -2994,7 +3003,7 @@
       <c r="V1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="37" t="s">
+      <c r="W1" s="17" t="s">
         <v>20</v>
       </c>
       <c r="X1" s="34" t="s">
@@ -3042,7 +3051,7 @@
       <c r="T2" s="47"/>
       <c r="U2" s="51"/>
       <c r="V2" s="51"/>
-      <c r="W2" s="48"/>
+      <c r="W2" s="68"/>
       <c r="X2" s="48"/>
       <c r="Y2" s="47"/>
       <c r="Z2" s="52"/>
@@ -3080,7 +3089,7 @@
       <c r="T3" s="58"/>
       <c r="U3" s="62"/>
       <c r="V3" s="62"/>
-      <c r="W3" s="57"/>
+      <c r="W3" s="69"/>
       <c r="X3" s="65"/>
       <c r="Y3" s="58"/>
       <c r="Z3" s="64"/>
@@ -3118,7 +3127,7 @@
       <c r="T4" s="58"/>
       <c r="U4" s="62"/>
       <c r="V4" s="62"/>
-      <c r="W4" s="57"/>
+      <c r="W4" s="69"/>
       <c r="X4" s="65"/>
       <c r="Y4" s="58"/>
       <c r="Z4" s="64"/>
@@ -3156,7 +3165,7 @@
       <c r="T5" s="58"/>
       <c r="U5" s="62"/>
       <c r="V5" s="62"/>
-      <c r="W5" s="57"/>
+      <c r="W5" s="69"/>
       <c r="X5" s="65"/>
       <c r="Y5" s="58"/>
       <c r="Z5" s="64"/>
@@ -3194,7 +3203,7 @@
       <c r="T6" s="58"/>
       <c r="U6" s="62"/>
       <c r="V6" s="62"/>
-      <c r="W6" s="57"/>
+      <c r="W6" s="69"/>
       <c r="X6" s="65"/>
       <c r="Y6" s="58"/>
       <c r="Z6" s="64"/>
@@ -3232,7 +3241,7 @@
       <c r="T7" s="58"/>
       <c r="U7" s="62"/>
       <c r="V7" s="62"/>
-      <c r="W7" s="57"/>
+      <c r="W7" s="69"/>
       <c r="X7" s="65"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="64"/>
@@ -3270,7 +3279,7 @@
       <c r="T8" s="58"/>
       <c r="U8" s="62"/>
       <c r="V8" s="62"/>
-      <c r="W8" s="57"/>
+      <c r="W8" s="69"/>
       <c r="X8" s="65"/>
       <c r="Y8" s="58"/>
       <c r="Z8" s="64"/>
@@ -3308,7 +3317,7 @@
       <c r="T9" s="58"/>
       <c r="U9" s="62"/>
       <c r="V9" s="62"/>
-      <c r="W9" s="57"/>
+      <c r="W9" s="69"/>
       <c r="X9" s="65"/>
       <c r="Y9" s="58"/>
       <c r="Z9" s="64"/>
@@ -3346,7 +3355,7 @@
       <c r="T10" s="58"/>
       <c r="U10" s="62"/>
       <c r="V10" s="62"/>
-      <c r="W10" s="57"/>
+      <c r="W10" s="69"/>
       <c r="X10" s="65"/>
       <c r="Y10" s="58"/>
       <c r="Z10" s="64"/>
@@ -3384,7 +3393,7 @@
       <c r="T11" s="58"/>
       <c r="U11" s="62"/>
       <c r="V11" s="62"/>
-      <c r="W11" s="57"/>
+      <c r="W11" s="69"/>
       <c r="X11" s="65"/>
       <c r="Y11" s="58"/>
       <c r="Z11" s="64"/>
@@ -3422,7 +3431,7 @@
       <c r="T12" s="58"/>
       <c r="U12" s="62"/>
       <c r="V12" s="62"/>
-      <c r="W12" s="57"/>
+      <c r="W12" s="69"/>
       <c r="X12" s="65"/>
       <c r="Y12" s="58"/>
       <c r="Z12" s="64"/>
@@ -3460,7 +3469,7 @@
       <c r="T13" s="58"/>
       <c r="U13" s="62"/>
       <c r="V13" s="62"/>
-      <c r="W13" s="57"/>
+      <c r="W13" s="69"/>
       <c r="X13" s="65"/>
       <c r="Y13" s="58"/>
       <c r="Z13" s="64"/>
@@ -3498,7 +3507,7 @@
       <c r="T14" s="58"/>
       <c r="U14" s="62"/>
       <c r="V14" s="62"/>
-      <c r="W14" s="57"/>
+      <c r="W14" s="69"/>
       <c r="X14" s="65"/>
       <c r="Y14" s="58"/>
       <c r="Z14" s="64"/>
@@ -3536,7 +3545,7 @@
       <c r="T15" s="58"/>
       <c r="U15" s="62"/>
       <c r="V15" s="62"/>
-      <c r="W15" s="57"/>
+      <c r="W15" s="69"/>
       <c r="X15" s="65"/>
       <c r="Y15" s="58"/>
       <c r="Z15" s="64"/>
@@ -3574,7 +3583,7 @@
       <c r="T16" s="58"/>
       <c r="U16" s="62"/>
       <c r="V16" s="62"/>
-      <c r="W16" s="57"/>
+      <c r="W16" s="69"/>
       <c r="X16" s="65"/>
       <c r="Y16" s="58"/>
       <c r="Z16" s="64"/>
@@ -3612,7 +3621,7 @@
       <c r="T17" s="58"/>
       <c r="U17" s="62"/>
       <c r="V17" s="62"/>
-      <c r="W17" s="57"/>
+      <c r="W17" s="69"/>
       <c r="X17" s="65"/>
       <c r="Y17" s="58"/>
       <c r="Z17" s="64"/>
@@ -3650,7 +3659,7 @@
       <c r="T18" s="58"/>
       <c r="U18" s="62"/>
       <c r="V18" s="62"/>
-      <c r="W18" s="57"/>
+      <c r="W18" s="69"/>
       <c r="X18" s="65"/>
       <c r="Y18" s="58"/>
       <c r="Z18" s="64"/>
@@ -3688,7 +3697,7 @@
       <c r="T19" s="58"/>
       <c r="U19" s="62"/>
       <c r="V19" s="62"/>
-      <c r="W19" s="57"/>
+      <c r="W19" s="69"/>
       <c r="X19" s="65"/>
       <c r="Y19" s="58"/>
       <c r="Z19" s="64"/>
@@ -3726,7 +3735,7 @@
       <c r="T20" s="58"/>
       <c r="U20" s="62"/>
       <c r="V20" s="62"/>
-      <c r="W20" s="57"/>
+      <c r="W20" s="69"/>
       <c r="X20" s="65"/>
       <c r="Y20" s="58"/>
       <c r="Z20" s="64"/>
@@ -3764,7 +3773,7 @@
       <c r="T21" s="58"/>
       <c r="U21" s="62"/>
       <c r="V21" s="62"/>
-      <c r="W21" s="57"/>
+      <c r="W21" s="69"/>
       <c r="X21" s="65"/>
       <c r="Y21" s="58"/>
       <c r="Z21" s="64"/>
@@ -3802,7 +3811,7 @@
       <c r="T22" s="58"/>
       <c r="U22" s="62"/>
       <c r="V22" s="62"/>
-      <c r="W22" s="57"/>
+      <c r="W22" s="69"/>
       <c r="X22" s="65"/>
       <c r="Y22" s="58"/>
       <c r="Z22" s="64"/>
@@ -3840,7 +3849,7 @@
       <c r="T23" s="58"/>
       <c r="U23" s="62"/>
       <c r="V23" s="62"/>
-      <c r="W23" s="57"/>
+      <c r="W23" s="69"/>
       <c r="X23" s="65"/>
       <c r="Y23" s="58"/>
       <c r="Z23" s="64"/>
@@ -3878,7 +3887,7 @@
       <c r="T24" s="58"/>
       <c r="U24" s="62"/>
       <c r="V24" s="62"/>
-      <c r="W24" s="57"/>
+      <c r="W24" s="69"/>
       <c r="X24" s="65"/>
       <c r="Y24" s="58"/>
       <c r="Z24" s="64"/>
@@ -3916,7 +3925,7 @@
       <c r="T25" s="58"/>
       <c r="U25" s="62"/>
       <c r="V25" s="62"/>
-      <c r="W25" s="57"/>
+      <c r="W25" s="69"/>
       <c r="X25" s="65"/>
       <c r="Y25" s="58"/>
       <c r="Z25" s="64"/>
@@ -3954,7 +3963,7 @@
       <c r="T26" s="58"/>
       <c r="U26" s="62"/>
       <c r="V26" s="62"/>
-      <c r="W26" s="57"/>
+      <c r="W26" s="69"/>
       <c r="X26" s="65"/>
       <c r="Y26" s="58"/>
       <c r="Z26" s="64"/>
@@ -3992,7 +4001,7 @@
       <c r="T27" s="58"/>
       <c r="U27" s="62"/>
       <c r="V27" s="62"/>
-      <c r="W27" s="57"/>
+      <c r="W27" s="69"/>
       <c r="X27" s="65"/>
       <c r="Y27" s="58"/>
       <c r="Z27" s="64"/>
@@ -4030,7 +4039,7 @@
       <c r="T28" s="58"/>
       <c r="U28" s="62"/>
       <c r="V28" s="62"/>
-      <c r="W28" s="57"/>
+      <c r="W28" s="69"/>
       <c r="X28" s="65"/>
       <c r="Y28" s="58"/>
       <c r="Z28" s="64"/>
@@ -4068,7 +4077,7 @@
       <c r="T29" s="58"/>
       <c r="U29" s="62"/>
       <c r="V29" s="62"/>
-      <c r="W29" s="57"/>
+      <c r="W29" s="69"/>
       <c r="X29" s="65"/>
       <c r="Y29" s="58"/>
       <c r="Z29" s="64"/>
@@ -4106,7 +4115,7 @@
       <c r="T30" s="58"/>
       <c r="U30" s="62"/>
       <c r="V30" s="62"/>
-      <c r="W30" s="57"/>
+      <c r="W30" s="69"/>
       <c r="X30" s="65"/>
       <c r="Y30" s="58"/>
       <c r="Z30" s="64"/>
@@ -4144,7 +4153,7 @@
       <c r="T31" s="58"/>
       <c r="U31" s="62"/>
       <c r="V31" s="62"/>
-      <c r="W31" s="57"/>
+      <c r="W31" s="69"/>
       <c r="X31" s="65"/>
       <c r="Y31" s="58"/>
       <c r="Z31" s="64"/>
@@ -4182,7 +4191,7 @@
       <c r="T32" s="58"/>
       <c r="U32" s="62"/>
       <c r="V32" s="62"/>
-      <c r="W32" s="57"/>
+      <c r="W32" s="69"/>
       <c r="X32" s="65"/>
       <c r="Y32" s="58"/>
       <c r="Z32" s="64"/>
@@ -4220,7 +4229,7 @@
       <c r="T33" s="58"/>
       <c r="U33" s="62"/>
       <c r="V33" s="62"/>
-      <c r="W33" s="57"/>
+      <c r="W33" s="69"/>
       <c r="X33" s="65"/>
       <c r="Y33" s="58"/>
       <c r="Z33" s="64"/>
@@ -4258,7 +4267,7 @@
       <c r="T34" s="58"/>
       <c r="U34" s="62"/>
       <c r="V34" s="62"/>
-      <c r="W34" s="57"/>
+      <c r="W34" s="69"/>
       <c r="X34" s="65"/>
       <c r="Y34" s="58"/>
       <c r="Z34" s="64"/>
@@ -4296,7 +4305,7 @@
       <c r="T35" s="58"/>
       <c r="U35" s="62"/>
       <c r="V35" s="62"/>
-      <c r="W35" s="57"/>
+      <c r="W35" s="69"/>
       <c r="X35" s="65"/>
       <c r="Y35" s="58"/>
       <c r="Z35" s="64"/>
@@ -4334,7 +4343,7 @@
       <c r="T36" s="58"/>
       <c r="U36" s="62"/>
       <c r="V36" s="62"/>
-      <c r="W36" s="57"/>
+      <c r="W36" s="69"/>
       <c r="X36" s="65"/>
       <c r="Y36" s="58"/>
       <c r="Z36" s="64"/>
@@ -4372,7 +4381,7 @@
       <c r="T37" s="58"/>
       <c r="U37" s="62"/>
       <c r="V37" s="62"/>
-      <c r="W37" s="57"/>
+      <c r="W37" s="69"/>
       <c r="X37" s="65"/>
       <c r="Y37" s="58"/>
       <c r="Z37" s="64"/>
@@ -4410,7 +4419,7 @@
       <c r="T38" s="58"/>
       <c r="U38" s="62"/>
       <c r="V38" s="62"/>
-      <c r="W38" s="57"/>
+      <c r="W38" s="69"/>
       <c r="X38" s="65"/>
       <c r="Y38" s="58"/>
       <c r="Z38" s="64"/>
@@ -4448,7 +4457,7 @@
       <c r="T39" s="58"/>
       <c r="U39" s="62"/>
       <c r="V39" s="62"/>
-      <c r="W39" s="57"/>
+      <c r="W39" s="69"/>
       <c r="X39" s="65"/>
       <c r="Y39" s="58"/>
       <c r="Z39" s="64"/>
@@ -4486,7 +4495,7 @@
       <c r="T40" s="58"/>
       <c r="U40" s="62"/>
       <c r="V40" s="62"/>
-      <c r="W40" s="57"/>
+      <c r="W40" s="69"/>
       <c r="X40" s="65"/>
       <c r="Y40" s="58"/>
       <c r="Z40" s="64"/>
@@ -4524,7 +4533,7 @@
       <c r="T41" s="58"/>
       <c r="U41" s="62"/>
       <c r="V41" s="62"/>
-      <c r="W41" s="57"/>
+      <c r="W41" s="69"/>
       <c r="X41" s="65"/>
       <c r="Y41" s="58"/>
       <c r="Z41" s="64"/>
@@ -4562,7 +4571,7 @@
       <c r="T42" s="58"/>
       <c r="U42" s="62"/>
       <c r="V42" s="62"/>
-      <c r="W42" s="57"/>
+      <c r="W42" s="69"/>
       <c r="X42" s="65"/>
       <c r="Y42" s="58"/>
       <c r="Z42" s="64"/>
@@ -4600,7 +4609,7 @@
       <c r="T43" s="58"/>
       <c r="U43" s="62"/>
       <c r="V43" s="62"/>
-      <c r="W43" s="57"/>
+      <c r="W43" s="69"/>
       <c r="X43" s="65"/>
       <c r="Y43" s="58"/>
       <c r="Z43" s="64"/>
@@ -4638,7 +4647,7 @@
       <c r="T44" s="58"/>
       <c r="U44" s="62"/>
       <c r="V44" s="62"/>
-      <c r="W44" s="57"/>
+      <c r="W44" s="69"/>
       <c r="X44" s="65"/>
       <c r="Y44" s="58"/>
       <c r="Z44" s="64"/>
@@ -4676,7 +4685,7 @@
       <c r="T45" s="58"/>
       <c r="U45" s="62"/>
       <c r="V45" s="62"/>
-      <c r="W45" s="57"/>
+      <c r="W45" s="69"/>
       <c r="X45" s="65"/>
       <c r="Y45" s="58"/>
       <c r="Z45" s="64"/>
@@ -4714,7 +4723,7 @@
       <c r="T46" s="58"/>
       <c r="U46" s="62"/>
       <c r="V46" s="62"/>
-      <c r="W46" s="57"/>
+      <c r="W46" s="69"/>
       <c r="X46" s="65"/>
       <c r="Y46" s="58"/>
       <c r="Z46" s="64"/>
@@ -4752,7 +4761,7 @@
       <c r="T47" s="58"/>
       <c r="U47" s="62"/>
       <c r="V47" s="62"/>
-      <c r="W47" s="57"/>
+      <c r="W47" s="69"/>
       <c r="X47" s="65"/>
       <c r="Y47" s="58"/>
       <c r="Z47" s="64"/>
@@ -4790,7 +4799,7 @@
       <c r="T48" s="58"/>
       <c r="U48" s="62"/>
       <c r="V48" s="62"/>
-      <c r="W48" s="57"/>
+      <c r="W48" s="69"/>
       <c r="X48" s="65"/>
       <c r="Y48" s="58"/>
       <c r="Z48" s="64"/>
@@ -4828,7 +4837,7 @@
       <c r="T49" s="58"/>
       <c r="U49" s="62"/>
       <c r="V49" s="62"/>
-      <c r="W49" s="57"/>
+      <c r="W49" s="69"/>
       <c r="X49" s="65"/>
       <c r="Y49" s="58"/>
       <c r="Z49" s="64"/>
@@ -4866,7 +4875,7 @@
       <c r="T50" s="58"/>
       <c r="U50" s="62"/>
       <c r="V50" s="62"/>
-      <c r="W50" s="57"/>
+      <c r="W50" s="69"/>
       <c r="X50" s="65"/>
       <c r="Y50" s="58"/>
       <c r="Z50" s="64"/>
@@ -4904,7 +4913,7 @@
       <c r="T51" s="58"/>
       <c r="U51" s="62"/>
       <c r="V51" s="62"/>
-      <c r="W51" s="57"/>
+      <c r="W51" s="69"/>
       <c r="X51" s="65"/>
       <c r="Y51" s="58"/>
       <c r="Z51" s="64"/>
@@ -4942,7 +4951,7 @@
       <c r="T52" s="58"/>
       <c r="U52" s="62"/>
       <c r="V52" s="62"/>
-      <c r="W52" s="57"/>
+      <c r="W52" s="69"/>
       <c r="X52" s="65"/>
       <c r="Y52" s="58"/>
       <c r="Z52" s="64"/>
@@ -4980,7 +4989,7 @@
       <c r="T53" s="58"/>
       <c r="U53" s="62"/>
       <c r="V53" s="62"/>
-      <c r="W53" s="57"/>
+      <c r="W53" s="69"/>
       <c r="X53" s="65"/>
       <c r="Y53" s="58"/>
       <c r="Z53" s="64"/>
@@ -5018,7 +5027,7 @@
       <c r="T54" s="58"/>
       <c r="U54" s="62"/>
       <c r="V54" s="62"/>
-      <c r="W54" s="57"/>
+      <c r="W54" s="69"/>
       <c r="X54" s="65"/>
       <c r="Y54" s="58"/>
       <c r="Z54" s="64"/>
@@ -5056,7 +5065,7 @@
       <c r="T55" s="58"/>
       <c r="U55" s="62"/>
       <c r="V55" s="62"/>
-      <c r="W55" s="57"/>
+      <c r="W55" s="69"/>
       <c r="X55" s="65"/>
       <c r="Y55" s="58"/>
       <c r="Z55" s="64"/>
@@ -5094,7 +5103,7 @@
       <c r="T56" s="58"/>
       <c r="U56" s="62"/>
       <c r="V56" s="62"/>
-      <c r="W56" s="57"/>
+      <c r="W56" s="69"/>
       <c r="X56" s="65"/>
       <c r="Y56" s="58"/>
       <c r="Z56" s="64"/>
@@ -5132,7 +5141,7 @@
       <c r="T57" s="58"/>
       <c r="U57" s="62"/>
       <c r="V57" s="62"/>
-      <c r="W57" s="57"/>
+      <c r="W57" s="69"/>
       <c r="X57" s="65"/>
       <c r="Y57" s="58"/>
       <c r="Z57" s="64"/>
@@ -5170,7 +5179,7 @@
       <c r="T58" s="58"/>
       <c r="U58" s="62"/>
       <c r="V58" s="62"/>
-      <c r="W58" s="57"/>
+      <c r="W58" s="69"/>
       <c r="X58" s="65"/>
       <c r="Y58" s="58"/>
       <c r="Z58" s="64"/>
@@ -5208,7 +5217,7 @@
       <c r="T59" s="58"/>
       <c r="U59" s="62"/>
       <c r="V59" s="62"/>
-      <c r="W59" s="57"/>
+      <c r="W59" s="69"/>
       <c r="X59" s="65"/>
       <c r="Y59" s="58"/>
       <c r="Z59" s="64"/>
@@ -5246,7 +5255,7 @@
       <c r="T60" s="58"/>
       <c r="U60" s="62"/>
       <c r="V60" s="62"/>
-      <c r="W60" s="57"/>
+      <c r="W60" s="69"/>
       <c r="X60" s="65"/>
       <c r="Y60" s="58"/>
       <c r="Z60" s="64"/>
@@ -5284,7 +5293,7 @@
       <c r="T61" s="58"/>
       <c r="U61" s="62"/>
       <c r="V61" s="62"/>
-      <c r="W61" s="57"/>
+      <c r="W61" s="69"/>
       <c r="X61" s="65"/>
       <c r="Y61" s="58"/>
       <c r="Z61" s="64"/>
@@ -5322,7 +5331,7 @@
       <c r="T62" s="58"/>
       <c r="U62" s="62"/>
       <c r="V62" s="62"/>
-      <c r="W62" s="57"/>
+      <c r="W62" s="69"/>
       <c r="X62" s="65"/>
       <c r="Y62" s="58"/>
       <c r="Z62" s="64"/>
@@ -5360,7 +5369,7 @@
       <c r="T63" s="58"/>
       <c r="U63" s="62"/>
       <c r="V63" s="62"/>
-      <c r="W63" s="57"/>
+      <c r="W63" s="69"/>
       <c r="X63" s="65"/>
       <c r="Y63" s="58"/>
       <c r="Z63" s="64"/>
@@ -5398,7 +5407,7 @@
       <c r="T64" s="58"/>
       <c r="U64" s="62"/>
       <c r="V64" s="62"/>
-      <c r="W64" s="57"/>
+      <c r="W64" s="69"/>
       <c r="X64" s="65"/>
       <c r="Y64" s="58"/>
       <c r="Z64" s="64"/>
@@ -5436,7 +5445,7 @@
       <c r="T65" s="58"/>
       <c r="U65" s="62"/>
       <c r="V65" s="62"/>
-      <c r="W65" s="57"/>
+      <c r="W65" s="69"/>
       <c r="X65" s="65"/>
       <c r="Y65" s="58"/>
       <c r="Z65" s="64"/>
@@ -5474,7 +5483,7 @@
       <c r="T66" s="58"/>
       <c r="U66" s="62"/>
       <c r="V66" s="62"/>
-      <c r="W66" s="57"/>
+      <c r="W66" s="69"/>
       <c r="X66" s="65"/>
       <c r="Y66" s="58"/>
       <c r="Z66" s="64"/>
@@ -5512,7 +5521,7 @@
       <c r="T67" s="58"/>
       <c r="U67" s="62"/>
       <c r="V67" s="62"/>
-      <c r="W67" s="57"/>
+      <c r="W67" s="69"/>
       <c r="X67" s="65"/>
       <c r="Y67" s="58"/>
       <c r="Z67" s="64"/>
@@ -5550,7 +5559,7 @@
       <c r="T68" s="58"/>
       <c r="U68" s="62"/>
       <c r="V68" s="62"/>
-      <c r="W68" s="57"/>
+      <c r="W68" s="69"/>
       <c r="X68" s="65"/>
       <c r="Y68" s="58"/>
       <c r="Z68" s="64"/>
@@ -5588,7 +5597,7 @@
       <c r="T69" s="58"/>
       <c r="U69" s="62"/>
       <c r="V69" s="62"/>
-      <c r="W69" s="57"/>
+      <c r="W69" s="69"/>
       <c r="X69" s="65"/>
       <c r="Y69" s="58"/>
       <c r="Z69" s="64"/>
@@ -5626,7 +5635,7 @@
       <c r="T70" s="58"/>
       <c r="U70" s="62"/>
       <c r="V70" s="62"/>
-      <c r="W70" s="57"/>
+      <c r="W70" s="69"/>
       <c r="X70" s="65"/>
       <c r="Y70" s="58"/>
       <c r="Z70" s="64"/>
@@ -5664,7 +5673,7 @@
       <c r="T71" s="58"/>
       <c r="U71" s="62"/>
       <c r="V71" s="62"/>
-      <c r="W71" s="57"/>
+      <c r="W71" s="69"/>
       <c r="X71" s="65"/>
       <c r="Y71" s="58"/>
       <c r="Z71" s="64"/>
@@ -5702,7 +5711,7 @@
       <c r="T72" s="58"/>
       <c r="U72" s="62"/>
       <c r="V72" s="62"/>
-      <c r="W72" s="57"/>
+      <c r="W72" s="69"/>
       <c r="X72" s="65"/>
       <c r="Y72" s="58"/>
       <c r="Z72" s="64"/>
@@ -5740,7 +5749,7 @@
       <c r="T73" s="58"/>
       <c r="U73" s="62"/>
       <c r="V73" s="62"/>
-      <c r="W73" s="57"/>
+      <c r="W73" s="69"/>
       <c r="X73" s="65"/>
       <c r="Y73" s="58"/>
       <c r="Z73" s="64"/>
@@ -5778,7 +5787,7 @@
       <c r="T74" s="58"/>
       <c r="U74" s="62"/>
       <c r="V74" s="62"/>
-      <c r="W74" s="57"/>
+      <c r="W74" s="69"/>
       <c r="X74" s="65"/>
       <c r="Y74" s="58"/>
       <c r="Z74" s="64"/>
@@ -5816,7 +5825,7 @@
       <c r="T75" s="58"/>
       <c r="U75" s="62"/>
       <c r="V75" s="62"/>
-      <c r="W75" s="57"/>
+      <c r="W75" s="69"/>
       <c r="X75" s="65"/>
       <c r="Y75" s="58"/>
       <c r="Z75" s="64"/>
@@ -5854,7 +5863,7 @@
       <c r="T76" s="58"/>
       <c r="U76" s="62"/>
       <c r="V76" s="62"/>
-      <c r="W76" s="57"/>
+      <c r="W76" s="69"/>
       <c r="X76" s="65"/>
       <c r="Y76" s="58"/>
       <c r="Z76" s="64"/>
@@ -5892,7 +5901,7 @@
       <c r="T77" s="58"/>
       <c r="U77" s="62"/>
       <c r="V77" s="62"/>
-      <c r="W77" s="57"/>
+      <c r="W77" s="69"/>
       <c r="X77" s="65"/>
       <c r="Y77" s="58"/>
       <c r="Z77" s="64"/>
@@ -5930,7 +5939,7 @@
       <c r="T78" s="58"/>
       <c r="U78" s="62"/>
       <c r="V78" s="62"/>
-      <c r="W78" s="57"/>
+      <c r="W78" s="69"/>
       <c r="X78" s="65"/>
       <c r="Y78" s="58"/>
       <c r="Z78" s="64"/>
@@ -5968,7 +5977,7 @@
       <c r="T79" s="58"/>
       <c r="U79" s="62"/>
       <c r="V79" s="62"/>
-      <c r="W79" s="57"/>
+      <c r="W79" s="69"/>
       <c r="X79" s="65"/>
       <c r="Y79" s="58"/>
       <c r="Z79" s="64"/>
@@ -6006,7 +6015,7 @@
       <c r="T80" s="58"/>
       <c r="U80" s="62"/>
       <c r="V80" s="62"/>
-      <c r="W80" s="57"/>
+      <c r="W80" s="69"/>
       <c r="X80" s="65"/>
       <c r="Y80" s="58"/>
       <c r="Z80" s="64"/>
@@ -6044,7 +6053,7 @@
       <c r="T81" s="58"/>
       <c r="U81" s="62"/>
       <c r="V81" s="62"/>
-      <c r="W81" s="57"/>
+      <c r="W81" s="69"/>
       <c r="X81" s="65"/>
       <c r="Y81" s="58"/>
       <c r="Z81" s="64"/>
@@ -6082,7 +6091,7 @@
       <c r="T82" s="58"/>
       <c r="U82" s="62"/>
       <c r="V82" s="62"/>
-      <c r="W82" s="57"/>
+      <c r="W82" s="69"/>
       <c r="X82" s="65"/>
       <c r="Y82" s="58"/>
       <c r="Z82" s="64"/>
@@ -6120,7 +6129,7 @@
       <c r="T83" s="58"/>
       <c r="U83" s="62"/>
       <c r="V83" s="62"/>
-      <c r="W83" s="57"/>
+      <c r="W83" s="69"/>
       <c r="X83" s="65"/>
       <c r="Y83" s="58"/>
       <c r="Z83" s="64"/>
@@ -6158,7 +6167,7 @@
       <c r="T84" s="58"/>
       <c r="U84" s="62"/>
       <c r="V84" s="62"/>
-      <c r="W84" s="57"/>
+      <c r="W84" s="69"/>
       <c r="X84" s="65"/>
       <c r="Y84" s="58"/>
       <c r="Z84" s="64"/>
@@ -6196,7 +6205,7 @@
       <c r="T85" s="58"/>
       <c r="U85" s="62"/>
       <c r="V85" s="62"/>
-      <c r="W85" s="57"/>
+      <c r="W85" s="69"/>
       <c r="X85" s="65"/>
       <c r="Y85" s="58"/>
       <c r="Z85" s="64"/>
@@ -6234,7 +6243,7 @@
       <c r="T86" s="58"/>
       <c r="U86" s="62"/>
       <c r="V86" s="62"/>
-      <c r="W86" s="57"/>
+      <c r="W86" s="69"/>
       <c r="X86" s="65"/>
       <c r="Y86" s="58"/>
       <c r="Z86" s="64"/>
@@ -6272,7 +6281,7 @@
       <c r="T87" s="58"/>
       <c r="U87" s="62"/>
       <c r="V87" s="62"/>
-      <c r="W87" s="57"/>
+      <c r="W87" s="69"/>
       <c r="X87" s="65"/>
       <c r="Y87" s="58"/>
       <c r="Z87" s="64"/>
@@ -6310,7 +6319,7 @@
       <c r="T88" s="58"/>
       <c r="U88" s="62"/>
       <c r="V88" s="62"/>
-      <c r="W88" s="57"/>
+      <c r="W88" s="69"/>
       <c r="X88" s="65"/>
       <c r="Y88" s="58"/>
       <c r="Z88" s="64"/>
@@ -6348,7 +6357,7 @@
       <c r="T89" s="58"/>
       <c r="U89" s="62"/>
       <c r="V89" s="62"/>
-      <c r="W89" s="57"/>
+      <c r="W89" s="69"/>
       <c r="X89" s="65"/>
       <c r="Y89" s="58"/>
       <c r="Z89" s="64"/>
@@ -6386,7 +6395,7 @@
       <c r="T90" s="58"/>
       <c r="U90" s="62"/>
       <c r="V90" s="62"/>
-      <c r="W90" s="57"/>
+      <c r="W90" s="69"/>
       <c r="X90" s="65"/>
       <c r="Y90" s="58"/>
       <c r="Z90" s="64"/>
@@ -6424,7 +6433,7 @@
       <c r="T91" s="58"/>
       <c r="U91" s="62"/>
       <c r="V91" s="62"/>
-      <c r="W91" s="57"/>
+      <c r="W91" s="69"/>
       <c r="X91" s="65"/>
       <c r="Y91" s="58"/>
       <c r="Z91" s="64"/>
@@ -6462,7 +6471,7 @@
       <c r="T92" s="58"/>
       <c r="U92" s="62"/>
       <c r="V92" s="62"/>
-      <c r="W92" s="57"/>
+      <c r="W92" s="69"/>
       <c r="X92" s="65"/>
       <c r="Y92" s="58"/>
       <c r="Z92" s="64"/>
@@ -6500,7 +6509,7 @@
       <c r="T93" s="58"/>
       <c r="U93" s="62"/>
       <c r="V93" s="62"/>
-      <c r="W93" s="57"/>
+      <c r="W93" s="69"/>
       <c r="X93" s="65"/>
       <c r="Y93" s="58"/>
       <c r="Z93" s="64"/>
@@ -6538,7 +6547,7 @@
       <c r="T94" s="58"/>
       <c r="U94" s="62"/>
       <c r="V94" s="62"/>
-      <c r="W94" s="57"/>
+      <c r="W94" s="69"/>
       <c r="X94" s="65"/>
       <c r="Y94" s="58"/>
       <c r="Z94" s="64"/>
@@ -6576,7 +6585,7 @@
       <c r="T95" s="58"/>
       <c r="U95" s="62"/>
       <c r="V95" s="62"/>
-      <c r="W95" s="57"/>
+      <c r="W95" s="69"/>
       <c r="X95" s="65"/>
       <c r="Y95" s="58"/>
       <c r="Z95" s="64"/>
@@ -6614,7 +6623,7 @@
       <c r="T96" s="58"/>
       <c r="U96" s="62"/>
       <c r="V96" s="62"/>
-      <c r="W96" s="57"/>
+      <c r="W96" s="69"/>
       <c r="X96" s="65"/>
       <c r="Y96" s="58"/>
       <c r="Z96" s="64"/>
@@ -6652,7 +6661,7 @@
       <c r="T97" s="58"/>
       <c r="U97" s="62"/>
       <c r="V97" s="62"/>
-      <c r="W97" s="57"/>
+      <c r="W97" s="69"/>
       <c r="X97" s="65"/>
       <c r="Y97" s="58"/>
       <c r="Z97" s="64"/>
@@ -6690,7 +6699,7 @@
       <c r="T98" s="58"/>
       <c r="U98" s="62"/>
       <c r="V98" s="62"/>
-      <c r="W98" s="57"/>
+      <c r="W98" s="69"/>
       <c r="X98" s="65"/>
       <c r="Y98" s="58"/>
       <c r="Z98" s="64"/>
@@ -6728,7 +6737,7 @@
       <c r="T99" s="58"/>
       <c r="U99" s="62"/>
       <c r="V99" s="62"/>
-      <c r="W99" s="57"/>
+      <c r="W99" s="69"/>
       <c r="X99" s="65"/>
       <c r="Y99" s="58"/>
       <c r="Z99" s="64"/>
@@ -6766,7 +6775,7 @@
       <c r="T100" s="58"/>
       <c r="U100" s="62"/>
       <c r="V100" s="62"/>
-      <c r="W100" s="57"/>
+      <c r="W100" s="69"/>
       <c r="X100" s="65"/>
       <c r="Y100" s="58"/>
       <c r="Z100" s="64"/>

</xml_diff>

<commit_message>
Alter allowable inputs for surgeons to include Not-Applicable
</commit_message>
<xml_diff>
--- a/doc/Batch_Upload_Template.xlsx
+++ b/doc/Batch_Upload_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmattioli\Projects\XNAT-Interact\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DE4112-ACA6-487D-B14B-E43E2877FEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17BE731-321E-450E-94F7-8294B2F34D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="3930" windowWidth="29040" windowHeight="15720" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
   </bookViews>
@@ -297,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="536">
   <si>
     <t>Quality</t>
   </si>
@@ -1948,6 +1948,9 @@
   </si>
   <si>
     <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>NOT-APPLICABLE</t>
   </si>
 </sst>
 </file>
@@ -2899,7 +2902,7 @@
   <dimension ref="A1:AK121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6911,9 +6914,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{08786D1C-564E-4A68-B1EA-1069F34FE29C}">
           <x14:formula1>
-            <xm:f>Allowable_Inputs!$F$2:$F$44</xm:f>
+            <xm:f>Allowable_Inputs!$F$2:$F$45</xm:f>
           </x14:formula1>
-          <xm:sqref>J101:J1048576 U1:U1048576 J1 L1:L2 L101:L1048576</xm:sqref>
+          <xm:sqref>J101:J1048576 L101:L1048576 L1:L2 J1 U1:U1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6925,8 +6928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DEE2E1-DFE1-4A7A-9865-D4F1FA133515}">
   <dimension ref="A1:XFC45"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F4:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6959,7 +6962,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>271</v>
       </c>
@@ -6982,7 +6985,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>272</v>
       </c>
@@ -6998,8 +7001,8 @@
       <c r="E3" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>224</v>
+      <c r="F3" s="33" t="s">
+        <v>535</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>280</v>
@@ -7021,8 +7024,8 @@
       <c r="E4" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>225</v>
+      <c r="F4" s="30" t="s">
+        <v>224</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>343</v>
@@ -7043,7 +7046,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G5" s="32"/>
     </row>
@@ -7058,7 +7061,7 @@
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G6" s="32"/>
     </row>
@@ -7073,7 +7076,7 @@
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G7" s="32"/>
     </row>
@@ -7088,7 +7091,7 @@
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G8" s="32"/>
     </row>
@@ -7101,7 +7104,7 @@
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G9" s="32"/>
     </row>
@@ -7114,7 +7117,7 @@
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G10" s="32"/>
     </row>
@@ -7127,7 +7130,7 @@
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G11" s="32"/>
     </row>
@@ -7140,7 +7143,7 @@
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G12" s="32"/>
     </row>
@@ -7153,7 +7156,7 @@
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G13" s="32"/>
     </row>
@@ -7166,7 +7169,7 @@
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G14" s="32"/>
     </row>
@@ -7179,7 +7182,7 @@
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G15" s="32"/>
     </row>
@@ -7192,7 +7195,7 @@
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G16" s="32"/>
     </row>
@@ -7205,7 +7208,7 @@
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G17" s="32"/>
     </row>
@@ -7218,7 +7221,7 @@
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G18" s="32"/>
     </row>
@@ -7231,7 +7234,7 @@
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G19" s="32"/>
     </row>
@@ -7244,7 +7247,7 @@
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G20" s="32"/>
     </row>
@@ -7257,7 +7260,7 @@
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G21" s="32"/>
     </row>
@@ -7270,7 +7273,7 @@
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G22" s="32"/>
     </row>
@@ -7283,7 +7286,7 @@
       </c>
       <c r="E23" s="32"/>
       <c r="F23" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G23" s="32"/>
     </row>
@@ -7296,7 +7299,7 @@
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G24" s="32"/>
     </row>
@@ -7309,7 +7312,7 @@
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G25" s="32"/>
     </row>
@@ -7322,7 +7325,7 @@
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G26" s="32"/>
     </row>
@@ -7335,7 +7338,7 @@
       </c>
       <c r="E27" s="32"/>
       <c r="F27" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G27" s="32"/>
     </row>
@@ -7348,7 +7351,7 @@
       </c>
       <c r="E28" s="32"/>
       <c r="F28" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G28" s="32"/>
     </row>
@@ -7361,7 +7364,7 @@
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G29" s="32"/>
     </row>
@@ -7372,7 +7375,7 @@
       <c r="D30" s="32"/>
       <c r="E30" s="32"/>
       <c r="F30" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G30" s="32"/>
     </row>
@@ -7383,7 +7386,7 @@
       <c r="D31" s="32"/>
       <c r="E31" s="32"/>
       <c r="F31" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G31" s="32"/>
     </row>
@@ -7394,7 +7397,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G32" s="32"/>
     </row>
@@ -7405,7 +7408,7 @@
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
       <c r="F33" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G33" s="32"/>
     </row>
@@ -7416,7 +7419,7 @@
       <c r="D34" s="32"/>
       <c r="E34" s="32"/>
       <c r="F34" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G34" s="32"/>
     </row>
@@ -7427,7 +7430,7 @@
       <c r="D35" s="32"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G35" s="32"/>
     </row>
@@ -7438,7 +7441,7 @@
       <c r="D36" s="32"/>
       <c r="E36" s="32"/>
       <c r="F36" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G36" s="32"/>
     </row>
@@ -7449,7 +7452,7 @@
       <c r="D37" s="32"/>
       <c r="E37" s="32"/>
       <c r="F37" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G37" s="32"/>
     </row>
@@ -7460,7 +7463,7 @@
       <c r="D38" s="32"/>
       <c r="E38" s="32"/>
       <c r="F38" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G38" s="32"/>
     </row>
@@ -7471,7 +7474,7 @@
       <c r="D39" s="32"/>
       <c r="E39" s="32"/>
       <c r="F39" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G39" s="32"/>
     </row>
@@ -7482,7 +7485,7 @@
       <c r="D40" s="32"/>
       <c r="E40" s="32"/>
       <c r="F40" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G40" s="32"/>
     </row>
@@ -7493,7 +7496,7 @@
       <c r="D41" s="32"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G41" s="32"/>
     </row>
@@ -7504,7 +7507,7 @@
       <c r="D42" s="32"/>
       <c r="E42" s="32"/>
       <c r="F42" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G42" s="32"/>
     </row>
@@ -7515,16 +7518,20 @@
       <c r="D43" s="32"/>
       <c r="E43" s="32"/>
       <c r="F43" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G43" s="32"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F44" s="32" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="32" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13128,9 +13135,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{69F90641-FF15-4066-B9EB-8A2C651BC207}">
           <x14:formula1>
-            <xm:f>Allowable_Inputs!$F$3:$F$44</xm:f>
+            <xm:f>Allowable_Inputs!$F$4:$F$45</xm:f>
           </x14:formula1>
-          <xm:sqref>K1:K23 V1:V1048576 K25:K35 K37:K1048576 M1:M1048576</xm:sqref>
+          <xm:sqref>K1:K23 M1:M1048576 K37:K1048576 K25:K35 V1:V1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
switch time column datatypes to be hh:mm in 24hr format
</commit_message>
<xml_diff>
--- a/doc/Batch_Upload_Template.xlsx
+++ b/doc/Batch_Upload_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmattioli\Projects\XNAT-Interact\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134A9FD9-633C-4988-B201-69E064E293AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB223A3-FB88-4BAD-B62D-BB31B79B2E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
+    <workbookView xWindow="-28920" yWindow="-1065" windowWidth="29040" windowHeight="15720" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -38,6 +38,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={4D708EE5-C8F9-495B-95BF-3788EE7DD0FE}</author>
     <author>tc={6DBB4B05-6E5D-4BC0-A924-70926B3D9DF4}</author>
     <author>tc={3BC687DA-6AF7-45BA-9AE2-DCFECB89CC73}</author>
     <author>tc={F97A624F-21D0-494A-AC12-39FA95E33169}</author>
@@ -53,7 +54,15 @@
     <author>tc={96F3B53C-E613-42DE-908F-C45C472CDC47}</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{6DBB4B05-6E5D-4BC0-A924-70926B3D9DF4}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4D708EE5-C8F9-495B-95BF-3788EE7DD0FE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    24hr format, e.g, 13:00 is 1pm</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{6DBB4B05-6E5D-4BC0-A924-70926B3D9DF4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,7 +70,7 @@
     Leave blank if unknown</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{3BC687DA-6AF7-45BA-9AE2-DCFECB89CC73}">
+    <comment ref="K1" authorId="2" shapeId="0" xr:uid="{3BC687DA-6AF7-45BA-9AE2-DCFECB89CC73}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -69,7 +78,7 @@
     You may leave this blank if Unknown. If a supervisor was the performer then leave this blank.</t>
       </text>
     </comment>
-    <comment ref="N1" authorId="2" shapeId="0" xr:uid="{F97A624F-21D0-494A-AC12-39FA95E33169}">
+    <comment ref="N1" authorId="3" shapeId="0" xr:uid="{F97A624F-21D0-494A-AC12-39FA95E33169}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -77,7 +86,7 @@
     e.g., 1 for PGY 1, or 15 years</t>
       </text>
     </comment>
-    <comment ref="P1" authorId="3" shapeId="0" xr:uid="{5B3D360B-2CD5-44DB-A18F-1D468FEC3BAE}">
+    <comment ref="P1" authorId="4" shapeId="0" xr:uid="{5B3D360B-2CD5-44DB-A18F-1D468FEC3BAE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -85,7 +94,7 @@
     cannot be left blank. must be at least 1</t>
       </text>
     </comment>
-    <comment ref="Q1" authorId="4" shapeId="0" xr:uid="{D40BC0A0-54DA-4550-87AF-BBC00133A174}">
+    <comment ref="Q1" authorId="5" shapeId="0" xr:uid="{D40BC0A0-54DA-4550-87AF-BBC00133A174}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -99,7 +108,7 @@
     {key1: task1; key2: task2; key3: task 3}</t>
       </text>
     </comment>
-    <comment ref="R1" authorId="5" shapeId="0" xr:uid="{D98BE6D6-47F7-4FEC-83E6-10761936D75B}">
+    <comment ref="R1" authorId="6" shapeId="0" xr:uid="{D98BE6D6-47F7-4FEC-83E6-10761936D75B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -107,7 +116,7 @@
     You may leave this blank</t>
       </text>
     </comment>
-    <comment ref="T1" authorId="6" shapeId="0" xr:uid="{AD2ECA50-3F1E-4AB5-8FD2-23CF9F38A8A8}">
+    <comment ref="T1" authorId="7" shapeId="0" xr:uid="{AD2ECA50-3F1E-4AB5-8FD2-23CF9F38A8A8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -115,7 +124,7 @@
     BMI, pre-existing conditions, etc.</t>
       </text>
     </comment>
-    <comment ref="U1" authorId="7" shapeId="0" xr:uid="{37C667C1-77C8-4B14-A0C9-78CB7B7DAB72}">
+    <comment ref="U1" authorId="8" shapeId="0" xr:uid="{37C667C1-77C8-4B14-A0C9-78CB7B7DAB72}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -123,7 +132,7 @@
     If none/unknown, leave blank. Otherwise, list the full name of the assessment</t>
       </text>
     </comment>
-    <comment ref="V1" authorId="8" shapeId="0" xr:uid="{DD2987B7-2B7D-4DC5-81E1-8D39B174E130}">
+    <comment ref="V1" authorId="9" shapeId="0" xr:uid="{DD2987B7-2B7D-4DC5-81E1-8D39B174E130}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -131,7 +140,7 @@
     Leave blank if none/unknown</t>
       </text>
     </comment>
-    <comment ref="W1" authorId="9" shapeId="0" xr:uid="{2A58B2F1-9692-462C-A6FC-3EAF16F139E7}">
+    <comment ref="W1" authorId="10" shapeId="0" xr:uid="{2A58B2F1-9692-462C-A6FC-3EAF16F139E7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -139,7 +148,7 @@
     Free form -- date of assessment; score; etc.</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="10" shapeId="0" xr:uid="{4A0C7026-6940-4C53-AE3C-9E947E817E0D}">
+    <comment ref="X1" authorId="11" shapeId="0" xr:uid="{4A0C7026-6940-4C53-AE3C-9E947E817E0D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -147,7 +156,7 @@
     e.g., usb drive; EPIC; etc. Optional field</t>
       </text>
     </comment>
-    <comment ref="Y1" authorId="11" shapeId="0" xr:uid="{ADEE9D98-136E-44EC-99E5-A9AFFD2594E1}">
+    <comment ref="Y1" authorId="12" shapeId="0" xr:uid="{ADEE9D98-136E-44EC-99E5-A9AFFD2594E1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -155,7 +164,7 @@
     Parent folder of the case data</t>
       </text>
     </comment>
-    <comment ref="Z1" authorId="12" shapeId="0" xr:uid="{96F3B53C-E613-42DE-908F-C45C472CDC47}">
+    <comment ref="Z1" authorId="13" shapeId="0" xr:uid="{96F3B53C-E613-42DE-908F-C45C472CDC47}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -607,12 +616,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,6 +656,12 @@
       <color rgb="FF3B3B3B"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -895,16 +909,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1234,6 +1248,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G1" dT="2024-12-13T17:08:48.42" personId="{09F1D53E-6429-4942-B85E-DCF0210217E4}" id="{4D708EE5-C8F9-495B-95BF-3788EE7DD0FE}">
+    <text>24hr format, e.g, 13:00 is 1pm</text>
+  </threadedComment>
   <threadedComment ref="H1" dT="2024-09-10T17:08:26.44" personId="{09F1D53E-6429-4942-B85E-DCF0210217E4}" id="{6DBB4B05-6E5D-4BC0-A924-70926B3D9DF4}">
     <text>Leave blank if unknown</text>
   </threadedComment>
@@ -1288,7 +1305,7 @@
   <dimension ref="A1:AL121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1445,7 @@
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="H2" s="52"/>
       <c r="I2" s="35"/>
       <c r="J2" s="35"/>
       <c r="K2" s="33"/>
@@ -1457,7 +1474,7 @@
       <c r="AH2" s="36"/>
       <c r="AI2" s="36"/>
       <c r="AJ2" s="38"/>
-      <c r="AK2" s="51"/>
+      <c r="AK2" s="52"/>
     </row>
     <row r="3" spans="1:37" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="40"/>
@@ -1465,7 +1482,7 @@
       <c r="D3" s="41"/>
       <c r="E3" s="40"/>
       <c r="F3" s="49"/>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="53"/>
       <c r="I3" s="42"/>
       <c r="J3" s="42"/>
@@ -1503,7 +1520,7 @@
       <c r="D4" s="41"/>
       <c r="E4" s="40"/>
       <c r="F4" s="49"/>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="53"/>
       <c r="I4" s="42"/>
       <c r="J4" s="42"/>
@@ -1541,7 +1558,7 @@
       <c r="D5" s="41"/>
       <c r="E5" s="40"/>
       <c r="F5" s="49"/>
-      <c r="G5" s="52"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="53"/>
       <c r="I5" s="42"/>
       <c r="J5" s="42"/>
@@ -1579,7 +1596,7 @@
       <c r="D6" s="41"/>
       <c r="E6" s="40"/>
       <c r="F6" s="49"/>
-      <c r="G6" s="52"/>
+      <c r="G6" s="51"/>
       <c r="H6" s="53"/>
       <c r="I6" s="42"/>
       <c r="J6" s="42"/>
@@ -1617,7 +1634,7 @@
       <c r="D7" s="41"/>
       <c r="E7" s="40"/>
       <c r="F7" s="49"/>
-      <c r="G7" s="52"/>
+      <c r="G7" s="51"/>
       <c r="H7" s="53"/>
       <c r="I7" s="42"/>
       <c r="J7" s="42"/>
@@ -1655,7 +1672,7 @@
       <c r="D8" s="41"/>
       <c r="E8" s="40"/>
       <c r="F8" s="49"/>
-      <c r="G8" s="52"/>
+      <c r="G8" s="51"/>
       <c r="H8" s="53"/>
       <c r="I8" s="42"/>
       <c r="J8" s="42"/>
@@ -1693,7 +1710,7 @@
       <c r="D9" s="41"/>
       <c r="E9" s="40"/>
       <c r="F9" s="49"/>
-      <c r="G9" s="52"/>
+      <c r="G9" s="51"/>
       <c r="H9" s="53"/>
       <c r="I9" s="42"/>
       <c r="J9" s="42"/>
@@ -1731,7 +1748,7 @@
       <c r="D10" s="41"/>
       <c r="E10" s="40"/>
       <c r="F10" s="49"/>
-      <c r="G10" s="52"/>
+      <c r="G10" s="51"/>
       <c r="H10" s="53"/>
       <c r="I10" s="42"/>
       <c r="J10" s="42"/>
@@ -1769,7 +1786,7 @@
       <c r="D11" s="41"/>
       <c r="E11" s="40"/>
       <c r="F11" s="49"/>
-      <c r="G11" s="52"/>
+      <c r="G11" s="51"/>
       <c r="H11" s="53"/>
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
@@ -1807,7 +1824,7 @@
       <c r="D12" s="41"/>
       <c r="E12" s="40"/>
       <c r="F12" s="49"/>
-      <c r="G12" s="52"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="53"/>
       <c r="I12" s="42"/>
       <c r="J12" s="42"/>
@@ -1845,7 +1862,7 @@
       <c r="D13" s="41"/>
       <c r="E13" s="40"/>
       <c r="F13" s="49"/>
-      <c r="G13" s="52"/>
+      <c r="G13" s="51"/>
       <c r="H13" s="53"/>
       <c r="I13" s="42"/>
       <c r="J13" s="42"/>
@@ -1883,7 +1900,7 @@
       <c r="D14" s="41"/>
       <c r="E14" s="40"/>
       <c r="F14" s="49"/>
-      <c r="G14" s="52"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="53"/>
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
@@ -1921,7 +1938,7 @@
       <c r="D15" s="41"/>
       <c r="E15" s="40"/>
       <c r="F15" s="49"/>
-      <c r="G15" s="52"/>
+      <c r="G15" s="51"/>
       <c r="H15" s="53"/>
       <c r="I15" s="42"/>
       <c r="J15" s="42"/>
@@ -1959,7 +1976,7 @@
       <c r="D16" s="41"/>
       <c r="E16" s="40"/>
       <c r="F16" s="49"/>
-      <c r="G16" s="52"/>
+      <c r="G16" s="51"/>
       <c r="H16" s="53"/>
       <c r="I16" s="42"/>
       <c r="J16" s="42"/>
@@ -1997,7 +2014,7 @@
       <c r="D17" s="41"/>
       <c r="E17" s="40"/>
       <c r="F17" s="49"/>
-      <c r="G17" s="52"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="53"/>
       <c r="I17" s="42"/>
       <c r="J17" s="42"/>
@@ -2035,7 +2052,7 @@
       <c r="D18" s="41"/>
       <c r="E18" s="40"/>
       <c r="F18" s="49"/>
-      <c r="G18" s="52"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="53"/>
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
@@ -2073,7 +2090,7 @@
       <c r="D19" s="41"/>
       <c r="E19" s="40"/>
       <c r="F19" s="49"/>
-      <c r="G19" s="52"/>
+      <c r="G19" s="51"/>
       <c r="H19" s="53"/>
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
@@ -2111,7 +2128,7 @@
       <c r="D20" s="41"/>
       <c r="E20" s="40"/>
       <c r="F20" s="49"/>
-      <c r="G20" s="52"/>
+      <c r="G20" s="51"/>
       <c r="H20" s="53"/>
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
@@ -2149,7 +2166,7 @@
       <c r="D21" s="41"/>
       <c r="E21" s="40"/>
       <c r="F21" s="49"/>
-      <c r="G21" s="52"/>
+      <c r="G21" s="51"/>
       <c r="H21" s="53"/>
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
@@ -2187,7 +2204,7 @@
       <c r="D22" s="41"/>
       <c r="E22" s="40"/>
       <c r="F22" s="49"/>
-      <c r="G22" s="52"/>
+      <c r="G22" s="51"/>
       <c r="H22" s="53"/>
       <c r="I22" s="42"/>
       <c r="J22" s="42"/>
@@ -2225,7 +2242,7 @@
       <c r="D23" s="41"/>
       <c r="E23" s="40"/>
       <c r="F23" s="49"/>
-      <c r="G23" s="52"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="53"/>
       <c r="I23" s="42"/>
       <c r="J23" s="42"/>
@@ -2263,7 +2280,7 @@
       <c r="D24" s="41"/>
       <c r="E24" s="40"/>
       <c r="F24" s="49"/>
-      <c r="G24" s="52"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="53"/>
       <c r="I24" s="42"/>
       <c r="J24" s="42"/>
@@ -2301,7 +2318,7 @@
       <c r="D25" s="41"/>
       <c r="E25" s="40"/>
       <c r="F25" s="49"/>
-      <c r="G25" s="52"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="53"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
@@ -2339,7 +2356,7 @@
       <c r="D26" s="41"/>
       <c r="E26" s="40"/>
       <c r="F26" s="49"/>
-      <c r="G26" s="52"/>
+      <c r="G26" s="51"/>
       <c r="H26" s="53"/>
       <c r="I26" s="42"/>
       <c r="J26" s="42"/>
@@ -2377,7 +2394,7 @@
       <c r="D27" s="41"/>
       <c r="E27" s="40"/>
       <c r="F27" s="49"/>
-      <c r="G27" s="52"/>
+      <c r="G27" s="51"/>
       <c r="H27" s="53"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
@@ -2415,7 +2432,7 @@
       <c r="D28" s="41"/>
       <c r="E28" s="40"/>
       <c r="F28" s="49"/>
-      <c r="G28" s="52"/>
+      <c r="G28" s="51"/>
       <c r="H28" s="53"/>
       <c r="I28" s="42"/>
       <c r="J28" s="42"/>
@@ -2453,7 +2470,7 @@
       <c r="D29" s="41"/>
       <c r="E29" s="40"/>
       <c r="F29" s="49"/>
-      <c r="G29" s="52"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="53"/>
       <c r="I29" s="42"/>
       <c r="J29" s="42"/>
@@ -2491,7 +2508,7 @@
       <c r="D30" s="41"/>
       <c r="E30" s="40"/>
       <c r="F30" s="49"/>
-      <c r="G30" s="52"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="53"/>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
@@ -2529,7 +2546,7 @@
       <c r="D31" s="41"/>
       <c r="E31" s="40"/>
       <c r="F31" s="49"/>
-      <c r="G31" s="52"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="53"/>
       <c r="I31" s="42"/>
       <c r="J31" s="42"/>
@@ -2567,7 +2584,7 @@
       <c r="D32" s="41"/>
       <c r="E32" s="40"/>
       <c r="F32" s="49"/>
-      <c r="G32" s="52"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="53"/>
       <c r="I32" s="42"/>
       <c r="J32" s="42"/>
@@ -2605,7 +2622,7 @@
       <c r="D33" s="41"/>
       <c r="E33" s="40"/>
       <c r="F33" s="49"/>
-      <c r="G33" s="52"/>
+      <c r="G33" s="51"/>
       <c r="H33" s="53"/>
       <c r="I33" s="42"/>
       <c r="J33" s="42"/>
@@ -2643,7 +2660,7 @@
       <c r="D34" s="41"/>
       <c r="E34" s="40"/>
       <c r="F34" s="49"/>
-      <c r="G34" s="52"/>
+      <c r="G34" s="51"/>
       <c r="H34" s="53"/>
       <c r="I34" s="42"/>
       <c r="J34" s="42"/>
@@ -2681,7 +2698,7 @@
       <c r="D35" s="41"/>
       <c r="E35" s="40"/>
       <c r="F35" s="49"/>
-      <c r="G35" s="52"/>
+      <c r="G35" s="51"/>
       <c r="H35" s="53"/>
       <c r="I35" s="42"/>
       <c r="J35" s="42"/>
@@ -2719,7 +2736,7 @@
       <c r="D36" s="41"/>
       <c r="E36" s="40"/>
       <c r="F36" s="49"/>
-      <c r="G36" s="52"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="53"/>
       <c r="I36" s="42"/>
       <c r="J36" s="42"/>
@@ -2757,7 +2774,7 @@
       <c r="D37" s="41"/>
       <c r="E37" s="40"/>
       <c r="F37" s="49"/>
-      <c r="G37" s="52"/>
+      <c r="G37" s="51"/>
       <c r="H37" s="53"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
@@ -2795,7 +2812,7 @@
       <c r="D38" s="41"/>
       <c r="E38" s="40"/>
       <c r="F38" s="49"/>
-      <c r="G38" s="52"/>
+      <c r="G38" s="51"/>
       <c r="H38" s="53"/>
       <c r="I38" s="42"/>
       <c r="J38" s="42"/>
@@ -2833,7 +2850,7 @@
       <c r="D39" s="41"/>
       <c r="E39" s="40"/>
       <c r="F39" s="49"/>
-      <c r="G39" s="52"/>
+      <c r="G39" s="51"/>
       <c r="H39" s="53"/>
       <c r="I39" s="42"/>
       <c r="J39" s="42"/>
@@ -2871,7 +2888,7 @@
       <c r="D40" s="41"/>
       <c r="E40" s="40"/>
       <c r="F40" s="49"/>
-      <c r="G40" s="52"/>
+      <c r="G40" s="51"/>
       <c r="H40" s="53"/>
       <c r="I40" s="42"/>
       <c r="J40" s="42"/>
@@ -2909,7 +2926,7 @@
       <c r="D41" s="41"/>
       <c r="E41" s="40"/>
       <c r="F41" s="49"/>
-      <c r="G41" s="52"/>
+      <c r="G41" s="51"/>
       <c r="H41" s="53"/>
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
@@ -2947,7 +2964,7 @@
       <c r="D42" s="41"/>
       <c r="E42" s="40"/>
       <c r="F42" s="49"/>
-      <c r="G42" s="52"/>
+      <c r="G42" s="51"/>
       <c r="H42" s="53"/>
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
@@ -2985,7 +3002,7 @@
       <c r="D43" s="41"/>
       <c r="E43" s="40"/>
       <c r="F43" s="49"/>
-      <c r="G43" s="52"/>
+      <c r="G43" s="51"/>
       <c r="H43" s="53"/>
       <c r="I43" s="42"/>
       <c r="J43" s="42"/>
@@ -3023,7 +3040,7 @@
       <c r="D44" s="41"/>
       <c r="E44" s="40"/>
       <c r="F44" s="49"/>
-      <c r="G44" s="52"/>
+      <c r="G44" s="51"/>
       <c r="H44" s="53"/>
       <c r="I44" s="42"/>
       <c r="J44" s="42"/>
@@ -3061,7 +3078,7 @@
       <c r="D45" s="41"/>
       <c r="E45" s="40"/>
       <c r="F45" s="49"/>
-      <c r="G45" s="52"/>
+      <c r="G45" s="51"/>
       <c r="H45" s="53"/>
       <c r="I45" s="42"/>
       <c r="J45" s="42"/>
@@ -3099,7 +3116,7 @@
       <c r="D46" s="41"/>
       <c r="E46" s="40"/>
       <c r="F46" s="49"/>
-      <c r="G46" s="52"/>
+      <c r="G46" s="51"/>
       <c r="H46" s="53"/>
       <c r="I46" s="42"/>
       <c r="J46" s="42"/>
@@ -3137,7 +3154,7 @@
       <c r="D47" s="41"/>
       <c r="E47" s="40"/>
       <c r="F47" s="49"/>
-      <c r="G47" s="52"/>
+      <c r="G47" s="51"/>
       <c r="H47" s="53"/>
       <c r="I47" s="42"/>
       <c r="J47" s="42"/>
@@ -3175,7 +3192,7 @@
       <c r="D48" s="41"/>
       <c r="E48" s="40"/>
       <c r="F48" s="49"/>
-      <c r="G48" s="52"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="53"/>
       <c r="I48" s="42"/>
       <c r="J48" s="42"/>
@@ -3213,7 +3230,7 @@
       <c r="D49" s="41"/>
       <c r="E49" s="40"/>
       <c r="F49" s="49"/>
-      <c r="G49" s="52"/>
+      <c r="G49" s="51"/>
       <c r="H49" s="53"/>
       <c r="I49" s="42"/>
       <c r="J49" s="42"/>
@@ -3251,7 +3268,7 @@
       <c r="D50" s="41"/>
       <c r="E50" s="40"/>
       <c r="F50" s="49"/>
-      <c r="G50" s="52"/>
+      <c r="G50" s="51"/>
       <c r="H50" s="53"/>
       <c r="I50" s="42"/>
       <c r="J50" s="42"/>
@@ -3289,7 +3306,7 @@
       <c r="D51" s="41"/>
       <c r="E51" s="40"/>
       <c r="F51" s="49"/>
-      <c r="G51" s="52"/>
+      <c r="G51" s="51"/>
       <c r="H51" s="53"/>
       <c r="I51" s="42"/>
       <c r="J51" s="42"/>
@@ -3327,7 +3344,7 @@
       <c r="D52" s="41"/>
       <c r="E52" s="40"/>
       <c r="F52" s="49"/>
-      <c r="G52" s="52"/>
+      <c r="G52" s="51"/>
       <c r="H52" s="53"/>
       <c r="I52" s="42"/>
       <c r="J52" s="42"/>
@@ -3365,7 +3382,7 @@
       <c r="D53" s="41"/>
       <c r="E53" s="40"/>
       <c r="F53" s="49"/>
-      <c r="G53" s="52"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="53"/>
       <c r="I53" s="42"/>
       <c r="J53" s="42"/>
@@ -3403,7 +3420,7 @@
       <c r="D54" s="41"/>
       <c r="E54" s="40"/>
       <c r="F54" s="49"/>
-      <c r="G54" s="52"/>
+      <c r="G54" s="51"/>
       <c r="H54" s="53"/>
       <c r="I54" s="42"/>
       <c r="J54" s="42"/>
@@ -3441,7 +3458,7 @@
       <c r="D55" s="41"/>
       <c r="E55" s="40"/>
       <c r="F55" s="49"/>
-      <c r="G55" s="52"/>
+      <c r="G55" s="51"/>
       <c r="H55" s="53"/>
       <c r="I55" s="42"/>
       <c r="J55" s="42"/>
@@ -3479,7 +3496,7 @@
       <c r="D56" s="41"/>
       <c r="E56" s="40"/>
       <c r="F56" s="49"/>
-      <c r="G56" s="52"/>
+      <c r="G56" s="51"/>
       <c r="H56" s="53"/>
       <c r="I56" s="42"/>
       <c r="J56" s="42"/>
@@ -3517,7 +3534,7 @@
       <c r="D57" s="41"/>
       <c r="E57" s="40"/>
       <c r="F57" s="49"/>
-      <c r="G57" s="52"/>
+      <c r="G57" s="51"/>
       <c r="H57" s="53"/>
       <c r="I57" s="42"/>
       <c r="J57" s="42"/>
@@ -3555,7 +3572,7 @@
       <c r="D58" s="41"/>
       <c r="E58" s="40"/>
       <c r="F58" s="49"/>
-      <c r="G58" s="52"/>
+      <c r="G58" s="51"/>
       <c r="H58" s="53"/>
       <c r="I58" s="42"/>
       <c r="J58" s="42"/>
@@ -3593,7 +3610,7 @@
       <c r="D59" s="41"/>
       <c r="E59" s="40"/>
       <c r="F59" s="49"/>
-      <c r="G59" s="52"/>
+      <c r="G59" s="51"/>
       <c r="H59" s="53"/>
       <c r="I59" s="42"/>
       <c r="J59" s="42"/>
@@ -3631,7 +3648,7 @@
       <c r="D60" s="41"/>
       <c r="E60" s="40"/>
       <c r="F60" s="49"/>
-      <c r="G60" s="52"/>
+      <c r="G60" s="51"/>
       <c r="H60" s="53"/>
       <c r="I60" s="42"/>
       <c r="J60" s="42"/>
@@ -3669,7 +3686,7 @@
       <c r="D61" s="41"/>
       <c r="E61" s="40"/>
       <c r="F61" s="49"/>
-      <c r="G61" s="52"/>
+      <c r="G61" s="51"/>
       <c r="H61" s="53"/>
       <c r="I61" s="42"/>
       <c r="J61" s="42"/>
@@ -3707,7 +3724,7 @@
       <c r="D62" s="41"/>
       <c r="E62" s="40"/>
       <c r="F62" s="49"/>
-      <c r="G62" s="52"/>
+      <c r="G62" s="51"/>
       <c r="H62" s="53"/>
       <c r="I62" s="42"/>
       <c r="J62" s="42"/>
@@ -3745,7 +3762,7 @@
       <c r="D63" s="41"/>
       <c r="E63" s="40"/>
       <c r="F63" s="49"/>
-      <c r="G63" s="52"/>
+      <c r="G63" s="51"/>
       <c r="H63" s="53"/>
       <c r="I63" s="42"/>
       <c r="J63" s="42"/>
@@ -3783,7 +3800,7 @@
       <c r="D64" s="41"/>
       <c r="E64" s="40"/>
       <c r="F64" s="49"/>
-      <c r="G64" s="52"/>
+      <c r="G64" s="51"/>
       <c r="H64" s="53"/>
       <c r="I64" s="42"/>
       <c r="J64" s="42"/>
@@ -3821,7 +3838,7 @@
       <c r="D65" s="41"/>
       <c r="E65" s="40"/>
       <c r="F65" s="49"/>
-      <c r="G65" s="52"/>
+      <c r="G65" s="51"/>
       <c r="H65" s="53"/>
       <c r="I65" s="42"/>
       <c r="J65" s="42"/>
@@ -3859,7 +3876,7 @@
       <c r="D66" s="41"/>
       <c r="E66" s="40"/>
       <c r="F66" s="49"/>
-      <c r="G66" s="52"/>
+      <c r="G66" s="51"/>
       <c r="H66" s="53"/>
       <c r="I66" s="42"/>
       <c r="J66" s="42"/>
@@ -3897,7 +3914,7 @@
       <c r="D67" s="41"/>
       <c r="E67" s="40"/>
       <c r="F67" s="49"/>
-      <c r="G67" s="52"/>
+      <c r="G67" s="51"/>
       <c r="H67" s="53"/>
       <c r="I67" s="42"/>
       <c r="J67" s="42"/>
@@ -3935,7 +3952,7 @@
       <c r="D68" s="41"/>
       <c r="E68" s="40"/>
       <c r="F68" s="49"/>
-      <c r="G68" s="52"/>
+      <c r="G68" s="51"/>
       <c r="H68" s="53"/>
       <c r="I68" s="42"/>
       <c r="J68" s="42"/>
@@ -3973,7 +3990,7 @@
       <c r="D69" s="41"/>
       <c r="E69" s="40"/>
       <c r="F69" s="49"/>
-      <c r="G69" s="52"/>
+      <c r="G69" s="51"/>
       <c r="H69" s="53"/>
       <c r="I69" s="42"/>
       <c r="J69" s="42"/>
@@ -4011,7 +4028,7 @@
       <c r="D70" s="41"/>
       <c r="E70" s="40"/>
       <c r="F70" s="49"/>
-      <c r="G70" s="52"/>
+      <c r="G70" s="51"/>
       <c r="H70" s="53"/>
       <c r="I70" s="42"/>
       <c r="J70" s="42"/>
@@ -4049,7 +4066,7 @@
       <c r="D71" s="41"/>
       <c r="E71" s="40"/>
       <c r="F71" s="49"/>
-      <c r="G71" s="52"/>
+      <c r="G71" s="51"/>
       <c r="H71" s="53"/>
       <c r="I71" s="42"/>
       <c r="J71" s="42"/>
@@ -4087,7 +4104,7 @@
       <c r="D72" s="41"/>
       <c r="E72" s="40"/>
       <c r="F72" s="49"/>
-      <c r="G72" s="52"/>
+      <c r="G72" s="51"/>
       <c r="H72" s="53"/>
       <c r="I72" s="42"/>
       <c r="J72" s="42"/>
@@ -4125,7 +4142,7 @@
       <c r="D73" s="41"/>
       <c r="E73" s="40"/>
       <c r="F73" s="49"/>
-      <c r="G73" s="52"/>
+      <c r="G73" s="51"/>
       <c r="H73" s="53"/>
       <c r="I73" s="42"/>
       <c r="J73" s="42"/>
@@ -4163,7 +4180,7 @@
       <c r="D74" s="41"/>
       <c r="E74" s="40"/>
       <c r="F74" s="49"/>
-      <c r="G74" s="52"/>
+      <c r="G74" s="51"/>
       <c r="H74" s="53"/>
       <c r="I74" s="42"/>
       <c r="J74" s="42"/>
@@ -4201,7 +4218,7 @@
       <c r="D75" s="41"/>
       <c r="E75" s="40"/>
       <c r="F75" s="49"/>
-      <c r="G75" s="52"/>
+      <c r="G75" s="51"/>
       <c r="H75" s="53"/>
       <c r="I75" s="42"/>
       <c r="J75" s="42"/>
@@ -4239,7 +4256,7 @@
       <c r="D76" s="41"/>
       <c r="E76" s="40"/>
       <c r="F76" s="49"/>
-      <c r="G76" s="52"/>
+      <c r="G76" s="51"/>
       <c r="H76" s="53"/>
       <c r="I76" s="42"/>
       <c r="J76" s="42"/>
@@ -4277,7 +4294,7 @@
       <c r="D77" s="41"/>
       <c r="E77" s="40"/>
       <c r="F77" s="49"/>
-      <c r="G77" s="52"/>
+      <c r="G77" s="51"/>
       <c r="H77" s="53"/>
       <c r="I77" s="42"/>
       <c r="J77" s="42"/>
@@ -4315,7 +4332,7 @@
       <c r="D78" s="41"/>
       <c r="E78" s="40"/>
       <c r="F78" s="49"/>
-      <c r="G78" s="52"/>
+      <c r="G78" s="51"/>
       <c r="H78" s="53"/>
       <c r="I78" s="42"/>
       <c r="J78" s="42"/>
@@ -4353,7 +4370,7 @@
       <c r="D79" s="41"/>
       <c r="E79" s="40"/>
       <c r="F79" s="49"/>
-      <c r="G79" s="52"/>
+      <c r="G79" s="51"/>
       <c r="H79" s="53"/>
       <c r="I79" s="42"/>
       <c r="J79" s="42"/>
@@ -4391,7 +4408,7 @@
       <c r="D80" s="41"/>
       <c r="E80" s="40"/>
       <c r="F80" s="49"/>
-      <c r="G80" s="52"/>
+      <c r="G80" s="51"/>
       <c r="H80" s="53"/>
       <c r="I80" s="42"/>
       <c r="J80" s="42"/>
@@ -4429,7 +4446,7 @@
       <c r="D81" s="41"/>
       <c r="E81" s="40"/>
       <c r="F81" s="49"/>
-      <c r="G81" s="52"/>
+      <c r="G81" s="51"/>
       <c r="H81" s="53"/>
       <c r="I81" s="42"/>
       <c r="J81" s="42"/>
@@ -4467,7 +4484,7 @@
       <c r="D82" s="41"/>
       <c r="E82" s="40"/>
       <c r="F82" s="49"/>
-      <c r="G82" s="52"/>
+      <c r="G82" s="51"/>
       <c r="H82" s="53"/>
       <c r="I82" s="42"/>
       <c r="J82" s="42"/>
@@ -4505,7 +4522,7 @@
       <c r="D83" s="41"/>
       <c r="E83" s="40"/>
       <c r="F83" s="49"/>
-      <c r="G83" s="52"/>
+      <c r="G83" s="51"/>
       <c r="H83" s="53"/>
       <c r="I83" s="42"/>
       <c r="J83" s="42"/>
@@ -4543,7 +4560,7 @@
       <c r="D84" s="41"/>
       <c r="E84" s="40"/>
       <c r="F84" s="49"/>
-      <c r="G84" s="52"/>
+      <c r="G84" s="51"/>
       <c r="H84" s="53"/>
       <c r="I84" s="42"/>
       <c r="J84" s="42"/>
@@ -4581,7 +4598,7 @@
       <c r="D85" s="41"/>
       <c r="E85" s="40"/>
       <c r="F85" s="49"/>
-      <c r="G85" s="52"/>
+      <c r="G85" s="51"/>
       <c r="H85" s="53"/>
       <c r="I85" s="42"/>
       <c r="J85" s="42"/>
@@ -4619,7 +4636,7 @@
       <c r="D86" s="41"/>
       <c r="E86" s="40"/>
       <c r="F86" s="49"/>
-      <c r="G86" s="52"/>
+      <c r="G86" s="51"/>
       <c r="H86" s="53"/>
       <c r="I86" s="42"/>
       <c r="J86" s="42"/>
@@ -4657,7 +4674,7 @@
       <c r="D87" s="41"/>
       <c r="E87" s="40"/>
       <c r="F87" s="49"/>
-      <c r="G87" s="52"/>
+      <c r="G87" s="51"/>
       <c r="H87" s="53"/>
       <c r="I87" s="42"/>
       <c r="J87" s="42"/>
@@ -4695,7 +4712,7 @@
       <c r="D88" s="41"/>
       <c r="E88" s="40"/>
       <c r="F88" s="49"/>
-      <c r="G88" s="52"/>
+      <c r="G88" s="51"/>
       <c r="H88" s="53"/>
       <c r="I88" s="42"/>
       <c r="J88" s="42"/>
@@ -4733,7 +4750,7 @@
       <c r="D89" s="41"/>
       <c r="E89" s="40"/>
       <c r="F89" s="49"/>
-      <c r="G89" s="52"/>
+      <c r="G89" s="51"/>
       <c r="H89" s="53"/>
       <c r="I89" s="42"/>
       <c r="J89" s="42"/>
@@ -4771,7 +4788,7 @@
       <c r="D90" s="41"/>
       <c r="E90" s="40"/>
       <c r="F90" s="49"/>
-      <c r="G90" s="52"/>
+      <c r="G90" s="51"/>
       <c r="H90" s="53"/>
       <c r="I90" s="42"/>
       <c r="J90" s="42"/>
@@ -4809,7 +4826,7 @@
       <c r="D91" s="41"/>
       <c r="E91" s="40"/>
       <c r="F91" s="49"/>
-      <c r="G91" s="52"/>
+      <c r="G91" s="51"/>
       <c r="H91" s="53"/>
       <c r="I91" s="42"/>
       <c r="J91" s="42"/>
@@ -4847,7 +4864,7 @@
       <c r="D92" s="41"/>
       <c r="E92" s="40"/>
       <c r="F92" s="49"/>
-      <c r="G92" s="52"/>
+      <c r="G92" s="51"/>
       <c r="H92" s="53"/>
       <c r="I92" s="42"/>
       <c r="J92" s="42"/>
@@ -4885,7 +4902,7 @@
       <c r="D93" s="41"/>
       <c r="E93" s="40"/>
       <c r="F93" s="49"/>
-      <c r="G93" s="52"/>
+      <c r="G93" s="51"/>
       <c r="H93" s="53"/>
       <c r="I93" s="42"/>
       <c r="J93" s="42"/>
@@ -4923,7 +4940,7 @@
       <c r="D94" s="41"/>
       <c r="E94" s="40"/>
       <c r="F94" s="49"/>
-      <c r="G94" s="52"/>
+      <c r="G94" s="51"/>
       <c r="H94" s="53"/>
       <c r="I94" s="42"/>
       <c r="J94" s="42"/>
@@ -4961,7 +4978,7 @@
       <c r="D95" s="41"/>
       <c r="E95" s="40"/>
       <c r="F95" s="49"/>
-      <c r="G95" s="52"/>
+      <c r="G95" s="51"/>
       <c r="H95" s="53"/>
       <c r="I95" s="42"/>
       <c r="J95" s="42"/>
@@ -4999,7 +5016,7 @@
       <c r="D96" s="41"/>
       <c r="E96" s="40"/>
       <c r="F96" s="49"/>
-      <c r="G96" s="52"/>
+      <c r="G96" s="51"/>
       <c r="H96" s="53"/>
       <c r="I96" s="42"/>
       <c r="J96" s="42"/>
@@ -5037,7 +5054,7 @@
       <c r="D97" s="41"/>
       <c r="E97" s="40"/>
       <c r="F97" s="49"/>
-      <c r="G97" s="52"/>
+      <c r="G97" s="51"/>
       <c r="H97" s="53"/>
       <c r="I97" s="42"/>
       <c r="J97" s="42"/>
@@ -5075,7 +5092,7 @@
       <c r="D98" s="41"/>
       <c r="E98" s="40"/>
       <c r="F98" s="49"/>
-      <c r="G98" s="52"/>
+      <c r="G98" s="51"/>
       <c r="H98" s="53"/>
       <c r="I98" s="42"/>
       <c r="J98" s="42"/>
@@ -5113,7 +5130,7 @@
       <c r="D99" s="41"/>
       <c r="E99" s="40"/>
       <c r="F99" s="49"/>
-      <c r="G99" s="52"/>
+      <c r="G99" s="51"/>
       <c r="H99" s="53"/>
       <c r="I99" s="42"/>
       <c r="J99" s="42"/>
@@ -5151,7 +5168,7 @@
       <c r="D100" s="41"/>
       <c r="E100" s="40"/>
       <c r="F100" s="49"/>
-      <c r="G100" s="52"/>
+      <c r="G100" s="51"/>
       <c r="H100" s="53"/>
       <c r="I100" s="42"/>
       <c r="J100" s="42"/>

</xml_diff>